<commit_message>
Subindo a atividade do Chart.Js
</commit_message>
<xml_diff>
--- a/Atividade de Gráficos - Pesquisa e Inovação.xlsx
+++ b/Atividade de Gráficos - Pesquisa e Inovação.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <xr:revisionPtr revIDLastSave="376" documentId="11_7F4755BF84DCCE43E268565A8931F45BFA75341E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{540E0360-D630-431C-B8E4-715C4033307E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráficos dos Sensores" sheetId="1" r:id="rId1"/>
@@ -3973,7 +3973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
@@ -4519,7 +4519,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>